<commit_message>
Monthly Update Real Estate
</commit_message>
<xml_diff>
--- a/images/Zillow/Tables/Zillow Summary Table.xlsx
+++ b/images/Zillow/Tables/Zillow Summary Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecnusbaum/Box/economic forecast project/frequent_releases/housing_update/output/Zillow/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecnusbaum/Box/economic_forecast_project/frequent_releases/housing_update/output/Zillow/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2DA351-2753-F943-9C1D-80849FDBC5DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9522269C-3ABD-934B-9D3D-5DDA1A7717A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15440" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1273,7 +1273,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1287,7 +1287,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="45">
-        <v>43929</v>
+        <v>43999</v>
       </c>
       <c r="B1" s="45"/>
     </row>
@@ -1324,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="13">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1373,16 +1373,16 @@
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="26">
-        <v>652059</v>
+        <v>658017</v>
       </c>
       <c r="D9" s="10">
-        <v>6.2654417676570899E-3</v>
+        <v>5.86382056342205E-3</v>
       </c>
       <c r="E9" s="30">
-        <v>2.1847056500521801E-2</v>
+        <v>2.54341619707774E-2</v>
       </c>
       <c r="F9" s="33">
-        <v>0.84518779099308405</v>
+        <v>0.84560412870327795</v>
       </c>
       <c r="G9" s="33">
         <v>2877</v>
@@ -1394,16 +1394,16 @@
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="26">
-        <v>571875</v>
+        <v>578267</v>
       </c>
       <c r="D10" s="10">
-        <v>9.4079022849022902E-3</v>
+        <v>7.4776775991984802E-3</v>
       </c>
       <c r="E10" s="30">
-        <v>3.8766068519053398E-2</v>
+        <v>4.3929500499157802E-2</v>
       </c>
       <c r="F10" s="33">
-        <v>1.0879097674560201</v>
+        <v>1.0914301892134199</v>
       </c>
       <c r="G10" s="33">
         <v>2657</v>
@@ -1415,16 +1415,16 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="26">
-        <v>247084</v>
+        <v>248857</v>
       </c>
       <c r="D11" s="40">
-        <v>3.86784327109035E-3</v>
+        <v>4.42361792211043E-3</v>
       </c>
       <c r="E11" s="31">
-        <v>3.86175529746067E-2</v>
+        <v>4.0554779685396197E-2</v>
       </c>
       <c r="F11" s="33">
-        <v>1.1572695849296999</v>
+        <v>1.1628614418422101</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>24</v>
@@ -1460,16 +1460,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="26">
-        <v>897325</v>
+        <v>903246</v>
       </c>
       <c r="D14" s="10">
-        <v>3.1750113193624902E-3</v>
+        <v>6.2228460664393E-3</v>
       </c>
       <c r="E14" s="30">
-        <v>3.1761328318897801E-3</v>
+        <v>1.1137393274577301E-2</v>
       </c>
       <c r="F14" s="33">
-        <v>0.92600523411088198</v>
+        <v>0.93132162160490095</v>
       </c>
       <c r="G14" s="33">
         <v>3853</v>
@@ -1481,16 +1481,16 @@
         <v>7</v>
       </c>
       <c r="C15" s="26">
-        <v>846130</v>
+        <v>856454</v>
       </c>
       <c r="D15" s="10">
-        <v>4.0380811342226597E-3</v>
+        <v>6.9828280512396201E-3</v>
       </c>
       <c r="E15" s="30">
-        <v>2.06449822982697E-2</v>
+        <v>3.0349110411476098E-2</v>
       </c>
       <c r="F15" s="33">
-        <v>0.83037691946090697</v>
+        <v>0.836244479660055</v>
       </c>
       <c r="G15" s="33">
         <v>3604</v>
@@ -1502,16 +1502,16 @@
         <v>8</v>
       </c>
       <c r="C16" s="26">
-        <v>366312</v>
+        <v>368496</v>
       </c>
       <c r="D16" s="40">
-        <v>5.4649608449690596E-3</v>
+        <v>6.5914014035068904E-3</v>
       </c>
       <c r="E16" s="31">
-        <v>2.29549948058041E-2</v>
+        <v>3.0936833800547101E-2</v>
       </c>
       <c r="F16" s="33">
-        <v>0.73006002917752899</v>
+        <v>0.73414791099281396</v>
       </c>
       <c r="G16" s="33">
         <v>1989</v>
@@ -1523,16 +1523,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="26">
-        <v>3387914</v>
+        <v>3276825</v>
       </c>
       <c r="D17" s="10">
-        <v>2.7362846138523399E-3</v>
+        <v>2.9984429278100402E-3</v>
       </c>
       <c r="E17" s="30">
-        <v>9.6228362283090597E-4</v>
+        <v>6.8745828790837101E-3</v>
       </c>
       <c r="F17" s="33">
-        <v>1.39438576735556</v>
+        <v>1.39801298340043</v>
       </c>
       <c r="G17" s="33">
         <v>10114</v>
@@ -1544,16 +1544,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="26">
-        <v>1133607</v>
+        <v>1134649</v>
       </c>
       <c r="D18" s="10">
-        <v>2.8645513102358898E-3</v>
+        <v>6.2673934135166797E-3</v>
       </c>
       <c r="E18" s="30">
-        <v>8.4071961542704406E-3</v>
+        <v>1.9905546407024102E-2</v>
       </c>
       <c r="F18" s="33">
-        <v>0.94392836980180606</v>
+        <v>0.95263878615584996</v>
       </c>
       <c r="G18" s="33">
         <v>4185</v>
@@ -1565,16 +1565,16 @@
         <v>10</v>
       </c>
       <c r="C19" s="26">
-        <v>408859</v>
+        <v>412599</v>
       </c>
       <c r="D19" s="40">
-        <v>5.4346623254943899E-3</v>
+        <v>5.8532708594385401E-3</v>
       </c>
       <c r="E19" s="31">
-        <v>3.4211578058047198E-2</v>
+        <v>3.9829130911427799E-2</v>
       </c>
       <c r="F19" s="33">
-        <v>0.81049165639161203</v>
+        <v>0.81380473372781104</v>
       </c>
       <c r="G19" s="33">
         <v>2117</v>
@@ -1586,16 +1586,16 @@
         <v>11</v>
       </c>
       <c r="C20" s="41">
-        <v>815110</v>
+        <v>813113</v>
       </c>
       <c r="D20" s="43">
-        <v>3.68049838850304E-6</v>
+        <v>1.62479643850544E-3</v>
       </c>
       <c r="E20" s="42">
-        <v>2.3683393523521399E-4</v>
+        <v>1.7025344603076599E-3</v>
       </c>
       <c r="F20" s="44">
-        <v>0.85122758649498198</v>
+        <v>0.85157613949245603</v>
       </c>
       <c r="G20" s="44">
         <v>3257</v>

</xml_diff>